<commit_message>
Add Gps simulation code and minimised the window on date 08-05-2020
</commit_message>
<xml_diff>
--- a/Read.xlsx
+++ b/Read.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="2" activeTab="11"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <t>Video Server</t>
   </si>
   <si>
-    <t>192.168.2.94</t>
+    <t>192.168.43.169</t>
   </si>
   <si>
     <t>10002</t>
@@ -108,7 +108,7 @@
     <t>LocationAction</t>
   </si>
   <si>
-    <t>First St</t>
+    <t>UatAutoTest</t>
   </si>
   <si>
     <t>India Test Location</t>
@@ -593,10 +593,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -615,6 +615,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -622,14 +629,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -658,10 +658,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -696,17 +720,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -728,6 +743,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -735,28 +757,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -785,13 +785,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,169 +965,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,6 +990,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1018,20 +1033,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1051,17 +1063,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1076,35 +1091,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1114,134 +1114,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1255,9 +1255,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
@@ -1706,7 +1703,7 @@
   <sheetPr/>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -1797,7 +1794,7 @@
       <c r="K2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1821,39 +1818,39 @@
     <col min="1" max="1" width="16.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="12.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="15.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="13.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="17.1111111111111" customWidth="1"/>
     <col min="10" max="10" width="22.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1870,13 +1867,13 @@
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1901,7 +1898,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1912,27 +1909,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1976,91 +1973,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2074,16 +2071,16 @@
       <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>65</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -2232,7 +2229,7 @@
       <c r="P1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>89</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -2307,7 +2304,7 @@
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -2414,7 +2411,7 @@
       <c r="Z1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="5" t="s">
         <v>126</v>
       </c>
       <c r="AB1" s="1" t="s">
@@ -2557,7 +2554,7 @@
       <c r="AJ2" t="s">
         <v>144</v>
       </c>
-      <c r="AK2" s="7" t="s">
+      <c r="AK2" s="6" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2695,8 +2692,8 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>

</xml_diff>

<commit_message>
committee the updated code for CDMP
</commit_message>
<xml_diff>
--- a/Read.xlsx
+++ b/Read.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="8"/>
+    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="193">
   <si>
     <t>UserName</t>
   </si>
@@ -36,10 +36,10 @@
     <t>WantToLogin</t>
   </si>
   <si>
-    <t>india_Uat_PE2</t>
-  </si>
-  <si>
-    <t>Vigilant1!</t>
+    <t>Uat_Demo_User2</t>
+  </si>
+  <si>
+    <t>Vigilant1!#</t>
   </si>
   <si>
     <t>yes</t>
@@ -81,7 +81,7 @@
     <t>Video Server</t>
   </si>
   <si>
-    <t>192.168.43.169</t>
+    <t>192.168.43.253</t>
   </si>
   <si>
     <t>10002</t>
@@ -108,7 +108,7 @@
     <t>LocationAction</t>
   </si>
   <si>
-    <t>UatAutoTest</t>
+    <t>California</t>
   </si>
   <si>
     <t>India Test Location</t>
@@ -222,7 +222,7 @@
     <t>2025</t>
   </si>
   <si>
-    <t>123</t>
+    <t>Amber Alert</t>
   </si>
   <si>
     <t>High Level</t>
@@ -435,9 +435,6 @@
     <t>C:\Program Files (x86)\Vigilant Solutions\Vigilant Mobile LPR\SOUND\BARK.wav</t>
   </si>
   <si>
-    <t>California</t>
-  </si>
-  <si>
     <t>http://learndev.vigilantsolutions.com/Learn52_Portal</t>
   </si>
   <si>
@@ -564,16 +561,19 @@
     <t>ExportIn</t>
   </si>
   <si>
-    <t>abcd</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Detections</t>
   </si>
   <si>
     <t>Last 24 Hours</t>
   </si>
   <si>
-    <t>12-04-2021</t>
-  </si>
-  <si>
-    <t>06:55:23 PM</t>
+    <t>02-07-2021</t>
+  </si>
+  <si>
+    <t>06:55:23 AM</t>
   </si>
   <si>
     <t>11-03-2021</t>
@@ -586,6 +586,24 @@
   </si>
   <si>
     <t>PDF</t>
+  </si>
+  <si>
+    <t>Hits</t>
+  </si>
+  <si>
+    <t>Last 25 Hours</t>
+  </si>
+  <si>
+    <t>02-07-2022</t>
+  </si>
+  <si>
+    <t>06:55:24 AM</t>
+  </si>
+  <si>
+    <t>11-03-2022</t>
+  </si>
+  <si>
+    <t>09:55:24 PM</t>
   </si>
 </sst>
 </file>
@@ -593,10 +611,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -615,7 +633,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -629,14 +647,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -658,9 +692,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -682,81 +769,12 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -785,13 +803,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,13 +893,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -821,19 +947,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -845,127 +977,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,17 +1012,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1034,21 +1046,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1072,11 +1069,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1091,12 +1094,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1114,138 +1132,141 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
@@ -1290,12 +1311,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1603,12 +1624,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="14.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="15.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="14.3333333333333" customWidth="1"/>
   </cols>
@@ -1625,13 +1646,13 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1654,11 +1675,11 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1684,12 +1705,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1701,13 +1722,13 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="29.1111111111111" customWidth="1"/>
     <col min="2" max="2" width="22.5555555555556" customWidth="1"/>
@@ -1724,77 +1745,115 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1810,7 +1869,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1823,66 +1882,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1898,41 +1957,42 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
+    <col min="1" max="1" width="17.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="19.1111111111111" customWidth="1"/>
     <col min="3" max="3" width="18.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="14.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1948,7 +2008,7 @@
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1973,180 +2033,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:29">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="K2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="T2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y2" s="2">
+      <c r="W2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="3">
         <v>1</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="3">
         <v>1</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AA2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2161,8 +2221,8 @@
   <sheetPr/>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -2229,7 +2289,7 @@
       <c r="P1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="8" t="s">
         <v>89</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -2237,58 +2297,58 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="J2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2303,8 +2363,8 @@
   <sheetPr/>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -2411,7 +2471,7 @@
       <c r="Z1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="6" t="s">
         <v>126</v>
       </c>
       <c r="AB1" s="1" t="s">
@@ -2446,116 +2506,116 @@
       </c>
     </row>
     <row r="2" spans="1:37">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>28</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="T2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="X2" s="3">
+        <v>8085</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="Q2" s="2">
-        <v>28</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="W2" s="3" t="s">
+      <c r="Z2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="X2" s="2">
-        <v>8085</v>
-      </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AA2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AB2" s="3">
+        <v>192</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>168</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>27</v>
+      </c>
+      <c r="AF2" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>192</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>168</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>5</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>27</v>
-      </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI2" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="AH2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" t="s">
         <v>143</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="AK2" s="6" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2585,60 +2645,60 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2663,22 +2723,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>161</v>
+      <c r="A2" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="3" t="s">
-        <v>162</v>
+      <c r="A3" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="3" t="s">
-        <v>163</v>
+      <c r="A4" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2692,7 +2752,7 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2703,11 +2763,11 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>